<commit_message>
add D_control - E_state
</commit_message>
<xml_diff>
--- a/CANID.xlsx
+++ b/CANID.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NEC-PCuser\Documents\Arduino\libraries\CCP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4959A7E6-CC3D-4079-B36C-BC58BDC3064A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FADDA27-9E02-4F49-955E-B137F3247361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="217">
   <si>
     <t>周波数が高いものは基本下の方に</t>
   </si>
@@ -828,6 +828,34 @@
     <t>FastLogger</t>
     <phoneticPr fontId="5"/>
   </si>
+  <si>
+    <t>CCP_D_control</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>CCP_D_state</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>CCP_E_control</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>(CHECK,DRAIN)</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>CCP_E_state</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>(STANDBY,)</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Valve</t>
+    <phoneticPr fontId="5"/>
+  </si>
 </sst>
 </file>
 
@@ -1181,8 +1209,8 @@
   </sheetPr>
   <dimension ref="A1:AD873"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2862,11 +2890,19 @@
         <f t="shared" si="2"/>
         <v>文字列</v>
       </c>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
+      <c r="E35" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="G35" s="9"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="9"/>
+      <c r="H35" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>161</v>
+      </c>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
       <c r="L35" s="9"/>
@@ -2905,11 +2941,19 @@
         <f t="shared" si="2"/>
         <v>文字列</v>
       </c>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
+      <c r="E36" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="G36" s="9"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="9"/>
+      <c r="H36" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>163</v>
+      </c>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
       <c r="L36" s="9"/>
@@ -2948,10 +2992,19 @@
         <f t="shared" si="2"/>
         <v>文字列</v>
       </c>
-      <c r="F37" s="9"/>
+      <c r="E37" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>213</v>
+      </c>
       <c r="G37" s="9"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="9"/>
+      <c r="H37" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>161</v>
+      </c>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
       <c r="L37" s="9"/>
@@ -2990,10 +3043,19 @@
         <f t="shared" si="2"/>
         <v>文字列</v>
       </c>
-      <c r="F38" s="9"/>
+      <c r="E38" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>215</v>
+      </c>
       <c r="G38" s="9"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="9"/>
+      <c r="H38" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>216</v>
+      </c>
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
       <c r="L38" s="9"/>

</xml_diff>

<commit_message>
add sensor kill command
</commit_message>
<xml_diff>
--- a/CANID.xlsx
+++ b/CANID.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NEC-PCuser\Documents\Arduino\libraries\CCP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8BAE96-322F-44AE-ACF6-20E3A59A4837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD528D6-8D29-4AF9-9F11-2D5180F762B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="375">
   <si>
     <t>周波数が高いものは基本下の方に</t>
   </si>
@@ -1647,6 +1647,14 @@
     <t>F(ADXL357)</t>
     <phoneticPr fontId="5"/>
   </si>
+  <si>
+    <t>o</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>(BEGIN,KILL)</t>
+    <phoneticPr fontId="5"/>
+  </si>
 </sst>
 </file>
 
@@ -1839,21 +1847,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1865,6 +1858,21 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2090,8 +2098,8 @@
   </sheetPr>
   <dimension ref="A1:AE987"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="V8" sqref="V8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2249,9 +2257,22 @@
         <v>196</v>
       </c>
       <c r="K4" s="9"/>
-      <c r="T4" s="9"/>
+      <c r="M4" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="T4" s="9" t="s">
+        <v>373</v>
+      </c>
       <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
+      <c r="V4" s="9" t="s">
+        <v>373</v>
+      </c>
       <c r="W4" s="9"/>
       <c r="X4" s="9"/>
       <c r="Y4" s="9"/>
@@ -3005,16 +3026,16 @@
       <c r="L18" s="18">
         <v>0</v>
       </c>
-      <c r="M18" s="23" t="s">
+      <c r="M18" s="24" t="s">
         <v>320</v>
       </c>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="23"/>
-      <c r="S18" s="23"/>
-      <c r="T18" s="23"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24"/>
+      <c r="S18" s="24"/>
+      <c r="T18" s="24"/>
       <c r="V18" s="9"/>
       <c r="W18" s="9"/>
       <c r="X18" s="9"/>
@@ -3059,7 +3080,7 @@
         <v>303</v>
       </c>
       <c r="K19" s="9"/>
-      <c r="L19" s="24">
+      <c r="L19" s="19">
         <v>1</v>
       </c>
       <c r="M19" s="15" t="s">
@@ -3120,7 +3141,7 @@
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
-      <c r="L20" s="25"/>
+      <c r="L20" s="20"/>
       <c r="M20" s="15">
         <v>1</v>
       </c>
@@ -3180,7 +3201,7 @@
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
-      <c r="L21" s="25"/>
+      <c r="L21" s="20"/>
       <c r="M21" s="15">
         <v>0</v>
       </c>
@@ -3240,7 +3261,7 @@
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
-      <c r="L22" s="25"/>
+      <c r="L22" s="20"/>
       <c r="M22" s="15">
         <v>0</v>
       </c>
@@ -3300,7 +3321,7 @@
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
-      <c r="L23" s="26"/>
+      <c r="L23" s="21"/>
       <c r="M23" s="15">
         <v>1</v>
       </c>
@@ -3360,7 +3381,7 @@
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
-      <c r="L24" s="27">
+      <c r="L24" s="22">
         <v>2</v>
       </c>
       <c r="M24" s="15" t="s">
@@ -3421,7 +3442,7 @@
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
-      <c r="L25" s="27"/>
+      <c r="L25" s="22"/>
       <c r="M25" s="15" t="s">
         <v>328</v>
       </c>
@@ -3480,7 +3501,7 @@
       <c r="I26" s="9"/>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
-      <c r="L26" s="27"/>
+      <c r="L26" s="22"/>
       <c r="M26" s="15" t="s">
         <v>327</v>
       </c>
@@ -3542,16 +3563,16 @@
       <c r="L27" s="16">
         <v>3</v>
       </c>
-      <c r="M27" s="27" t="s">
+      <c r="M27" s="22" t="s">
         <v>322</v>
       </c>
-      <c r="N27" s="27"/>
-      <c r="O27" s="27"/>
-      <c r="P27" s="27"/>
-      <c r="Q27" s="27"/>
-      <c r="R27" s="27"/>
-      <c r="S27" s="27"/>
-      <c r="T27" s="27"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="22"/>
       <c r="V27" s="9"/>
       <c r="W27" s="9"/>
       <c r="X27" s="9"/>
@@ -3589,14 +3610,14 @@
       <c r="L28" s="16">
         <v>4</v>
       </c>
-      <c r="M28" s="27"/>
-      <c r="N28" s="27"/>
-      <c r="O28" s="27"/>
-      <c r="P28" s="27"/>
-      <c r="Q28" s="27"/>
-      <c r="R28" s="27"/>
-      <c r="S28" s="27"/>
-      <c r="T28" s="27"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22"/>
       <c r="V28" s="9"/>
       <c r="W28" s="9"/>
       <c r="X28" s="9"/>
@@ -3628,7 +3649,7 @@
         <v>44</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>45</v>
+        <v>374</v>
       </c>
       <c r="G29" s="9"/>
       <c r="H29" s="8" t="s">
@@ -3642,16 +3663,16 @@
       <c r="L29" s="16">
         <v>5</v>
       </c>
-      <c r="M29" s="19" t="s">
+      <c r="M29" s="23" t="s">
         <v>323</v>
       </c>
-      <c r="N29" s="19"/>
-      <c r="O29" s="19"/>
-      <c r="P29" s="19"/>
-      <c r="Q29" s="19"/>
-      <c r="R29" s="19"/>
-      <c r="S29" s="19"/>
-      <c r="T29" s="19"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="23"/>
+      <c r="R29" s="23"/>
+      <c r="S29" s="23"/>
+      <c r="T29" s="23"/>
       <c r="V29" s="9"/>
       <c r="W29" s="9"/>
       <c r="X29" s="9"/>
@@ -3699,14 +3720,14 @@
       <c r="L30" s="16">
         <v>6</v>
       </c>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
-      <c r="O30" s="19"/>
-      <c r="P30" s="19"/>
-      <c r="Q30" s="19"/>
-      <c r="R30" s="19"/>
-      <c r="S30" s="19"/>
-      <c r="T30" s="19"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="23"/>
+      <c r="P30" s="23"/>
+      <c r="Q30" s="23"/>
+      <c r="R30" s="23"/>
+      <c r="S30" s="23"/>
+      <c r="T30" s="23"/>
       <c r="V30" s="9"/>
       <c r="W30" s="9"/>
       <c r="X30" s="9"/>
@@ -4006,10 +4027,10 @@
       <c r="L36" s="14">
         <v>3</v>
       </c>
-      <c r="M36" s="19" t="s">
+      <c r="M36" s="23" t="s">
         <v>306</v>
       </c>
-      <c r="N36" s="19" t="s">
+      <c r="N36" s="23" t="s">
         <v>307</v>
       </c>
       <c r="V36" s="9"/>
@@ -4057,8 +4078,8 @@
       <c r="L37" s="14">
         <v>4</v>
       </c>
-      <c r="M37" s="19"/>
-      <c r="N37" s="19"/>
+      <c r="M37" s="23"/>
+      <c r="N37" s="23"/>
       <c r="V37" s="9"/>
       <c r="W37" s="9"/>
       <c r="X37" s="9"/>
@@ -4106,10 +4127,10 @@
       <c r="L38" s="14">
         <v>5</v>
       </c>
-      <c r="M38" s="19" t="s">
+      <c r="M38" s="23" t="s">
         <v>308</v>
       </c>
-      <c r="N38" s="19" t="s">
+      <c r="N38" s="23" t="s">
         <v>310</v>
       </c>
       <c r="V38" s="9"/>
@@ -4157,8 +4178,8 @@
       <c r="L39" s="14">
         <v>6</v>
       </c>
-      <c r="M39" s="19"/>
-      <c r="N39" s="19"/>
+      <c r="M39" s="23"/>
+      <c r="N39" s="23"/>
       <c r="V39" s="9"/>
       <c r="W39" s="9"/>
       <c r="X39" s="9"/>
@@ -4206,10 +4227,10 @@
       <c r="L40" s="14">
         <v>7</v>
       </c>
-      <c r="M40" s="19" t="s">
+      <c r="M40" s="23" t="s">
         <v>308</v>
       </c>
-      <c r="N40" s="19" t="s">
+      <c r="N40" s="23" t="s">
         <v>309</v>
       </c>
       <c r="V40" s="9"/>
@@ -4255,8 +4276,8 @@
       <c r="L41" s="14">
         <v>8</v>
       </c>
-      <c r="M41" s="19"/>
-      <c r="N41" s="19"/>
+      <c r="M41" s="23"/>
+      <c r="N41" s="23"/>
       <c r="V41" s="9"/>
       <c r="W41" s="9"/>
       <c r="X41" s="9"/>
@@ -4300,10 +4321,10 @@
       <c r="L42" s="14">
         <v>9</v>
       </c>
-      <c r="M42" s="19" t="s">
+      <c r="M42" s="23" t="s">
         <v>308</v>
       </c>
-      <c r="N42" s="19" t="s">
+      <c r="N42" s="23" t="s">
         <v>359</v>
       </c>
       <c r="V42" s="9"/>
@@ -4343,8 +4364,8 @@
       <c r="L43" s="14">
         <v>10</v>
       </c>
-      <c r="M43" s="19"/>
-      <c r="N43" s="19"/>
+      <c r="M43" s="23"/>
+      <c r="N43" s="23"/>
       <c r="V43" s="9"/>
       <c r="W43" s="9"/>
       <c r="X43" s="9"/>
@@ -4382,10 +4403,10 @@
       <c r="L44" s="14">
         <v>11</v>
       </c>
-      <c r="M44" s="19" t="s">
+      <c r="M44" s="23" t="s">
         <v>343</v>
       </c>
-      <c r="N44" s="19" t="s">
+      <c r="N44" s="23" t="s">
         <v>316</v>
       </c>
       <c r="V44" s="9"/>
@@ -4433,8 +4454,8 @@
       <c r="L45" s="14">
         <v>12</v>
       </c>
-      <c r="M45" s="19"/>
-      <c r="N45" s="19"/>
+      <c r="M45" s="23"/>
+      <c r="N45" s="23"/>
       <c r="U45" s="9"/>
       <c r="V45" s="9"/>
       <c r="W45" s="9"/>
@@ -4483,8 +4504,8 @@
       <c r="L46" s="14">
         <v>13</v>
       </c>
-      <c r="M46" s="19"/>
-      <c r="N46" s="19"/>
+      <c r="M46" s="23"/>
+      <c r="N46" s="23"/>
       <c r="T46" s="9"/>
       <c r="U46" s="9"/>
       <c r="V46" s="9"/>
@@ -4532,8 +4553,8 @@
       <c r="L47" s="14">
         <v>14</v>
       </c>
-      <c r="M47" s="19"/>
-      <c r="N47" s="19"/>
+      <c r="M47" s="23"/>
+      <c r="N47" s="23"/>
       <c r="T47" s="9"/>
       <c r="U47" s="9"/>
       <c r="V47" s="9"/>
@@ -4583,10 +4604,10 @@
       <c r="L48" s="14">
         <v>15</v>
       </c>
-      <c r="M48" s="19" t="s">
+      <c r="M48" s="23" t="s">
         <v>343</v>
       </c>
-      <c r="N48" s="19" t="s">
+      <c r="N48" s="23" t="s">
         <v>319</v>
       </c>
       <c r="T48" s="9"/>
@@ -4636,8 +4657,8 @@
       <c r="L49" s="14">
         <v>16</v>
       </c>
-      <c r="M49" s="19"/>
-      <c r="N49" s="19"/>
+      <c r="M49" s="23"/>
+      <c r="N49" s="23"/>
       <c r="T49" s="9"/>
       <c r="U49" s="9"/>
       <c r="V49" s="9"/>
@@ -4687,8 +4708,8 @@
       <c r="L50" s="14">
         <v>17</v>
       </c>
-      <c r="M50" s="19"/>
-      <c r="N50" s="19"/>
+      <c r="M50" s="23"/>
+      <c r="N50" s="23"/>
       <c r="T50" s="9"/>
       <c r="U50" s="9"/>
       <c r="V50" s="9"/>
@@ -4736,8 +4757,8 @@
       <c r="L51" s="14">
         <v>18</v>
       </c>
-      <c r="M51" s="19"/>
-      <c r="N51" s="19"/>
+      <c r="M51" s="23"/>
+      <c r="N51" s="23"/>
       <c r="T51" s="9"/>
       <c r="U51" s="9"/>
       <c r="V51" s="9"/>
@@ -4787,10 +4808,10 @@
       <c r="L52" s="14">
         <v>19</v>
       </c>
-      <c r="M52" s="19" t="s">
+      <c r="M52" s="23" t="s">
         <v>308</v>
       </c>
-      <c r="N52" s="19" t="s">
+      <c r="N52" s="23" t="s">
         <v>317</v>
       </c>
       <c r="T52" s="9"/>
@@ -4840,8 +4861,8 @@
       <c r="L53" s="14">
         <v>20</v>
       </c>
-      <c r="M53" s="19"/>
-      <c r="N53" s="19"/>
+      <c r="M53" s="23"/>
+      <c r="N53" s="23"/>
       <c r="T53" s="9"/>
       <c r="U53" s="9"/>
       <c r="V53" s="9"/>
@@ -4891,10 +4912,10 @@
       <c r="L54" s="14">
         <v>21</v>
       </c>
-      <c r="M54" s="19" t="s">
+      <c r="M54" s="23" t="s">
         <v>308</v>
       </c>
-      <c r="N54" s="19" t="s">
+      <c r="N54" s="23" t="s">
         <v>318</v>
       </c>
       <c r="T54" s="9"/>
@@ -4936,8 +4957,8 @@
       <c r="L55" s="14">
         <v>22</v>
       </c>
-      <c r="M55" s="19"/>
-      <c r="N55" s="19"/>
+      <c r="M55" s="23"/>
+      <c r="N55" s="23"/>
       <c r="T55" s="9"/>
       <c r="U55" s="9"/>
       <c r="V55" s="9"/>
@@ -4977,10 +4998,10 @@
       <c r="L56" s="14">
         <v>23</v>
       </c>
-      <c r="M56" s="19" t="s">
+      <c r="M56" s="23" t="s">
         <v>308</v>
       </c>
-      <c r="N56" s="20" t="s">
+      <c r="N56" s="25" t="s">
         <v>358</v>
       </c>
       <c r="T56" s="9"/>
@@ -5022,8 +5043,8 @@
       <c r="L57" s="14">
         <v>24</v>
       </c>
-      <c r="M57" s="19"/>
-      <c r="N57" s="21"/>
+      <c r="M57" s="23"/>
+      <c r="N57" s="26"/>
       <c r="S57" s="9"/>
       <c r="T57" s="9"/>
       <c r="U57" s="9"/>
@@ -5064,10 +5085,10 @@
       <c r="L58" s="14">
         <v>25</v>
       </c>
-      <c r="M58" s="19" t="s">
+      <c r="M58" s="23" t="s">
         <v>311</v>
       </c>
-      <c r="N58" s="19" t="s">
+      <c r="N58" s="23" t="s">
         <v>314</v>
       </c>
       <c r="S58" s="9"/>
@@ -5118,8 +5139,8 @@
       <c r="L59" s="14">
         <v>26</v>
       </c>
-      <c r="M59" s="19"/>
-      <c r="N59" s="19"/>
+      <c r="M59" s="23"/>
+      <c r="N59" s="23"/>
       <c r="S59" s="9"/>
       <c r="T59" s="9"/>
       <c r="U59" s="9"/>
@@ -5168,8 +5189,8 @@
       <c r="L60" s="14">
         <v>27</v>
       </c>
-      <c r="M60" s="19"/>
-      <c r="N60" s="19"/>
+      <c r="M60" s="23"/>
+      <c r="N60" s="23"/>
       <c r="S60" s="9"/>
       <c r="T60" s="9"/>
       <c r="U60" s="9"/>
@@ -5210,8 +5231,8 @@
       <c r="L61" s="14">
         <v>28</v>
       </c>
-      <c r="M61" s="19"/>
-      <c r="N61" s="19"/>
+      <c r="M61" s="23"/>
+      <c r="N61" s="23"/>
       <c r="S61" s="9"/>
       <c r="T61" s="9"/>
       <c r="U61" s="9"/>
@@ -5264,10 +5285,10 @@
       <c r="L62" s="14">
         <v>29</v>
       </c>
-      <c r="M62" s="19" t="s">
+      <c r="M62" s="23" t="s">
         <v>311</v>
       </c>
-      <c r="N62" s="19" t="s">
+      <c r="N62" s="23" t="s">
         <v>315</v>
       </c>
       <c r="S62" s="9"/>
@@ -5320,8 +5341,8 @@
       <c r="L63" s="14">
         <v>30</v>
       </c>
-      <c r="M63" s="19"/>
-      <c r="N63" s="19"/>
+      <c r="M63" s="23"/>
+      <c r="N63" s="23"/>
       <c r="S63" s="9"/>
       <c r="T63" s="9"/>
       <c r="U63" s="9"/>
@@ -5372,8 +5393,8 @@
       <c r="L64" s="14">
         <v>31</v>
       </c>
-      <c r="M64" s="19"/>
-      <c r="N64" s="19"/>
+      <c r="M64" s="23"/>
+      <c r="N64" s="23"/>
       <c r="S64" s="9"/>
       <c r="T64" s="9"/>
       <c r="U64" s="9"/>
@@ -5421,8 +5442,8 @@
       <c r="L65" s="14">
         <v>32</v>
       </c>
-      <c r="M65" s="19"/>
-      <c r="N65" s="19"/>
+      <c r="M65" s="23"/>
+      <c r="N65" s="23"/>
       <c r="S65" s="9"/>
       <c r="T65" s="9"/>
       <c r="U65" s="9"/>
@@ -5473,10 +5494,10 @@
       <c r="L66" s="14">
         <v>33</v>
       </c>
-      <c r="M66" s="19" t="s">
+      <c r="M66" s="23" t="s">
         <v>308</v>
       </c>
-      <c r="N66" s="19" t="s">
+      <c r="N66" s="23" t="s">
         <v>360</v>
       </c>
       <c r="S66" s="9"/>
@@ -5527,8 +5548,8 @@
       <c r="L67" s="14">
         <v>34</v>
       </c>
-      <c r="M67" s="19"/>
-      <c r="N67" s="19"/>
+      <c r="M67" s="23"/>
+      <c r="N67" s="23"/>
       <c r="S67" s="9"/>
       <c r="T67" s="9"/>
       <c r="U67" s="9"/>
@@ -5577,10 +5598,10 @@
       <c r="L68" s="14">
         <v>35</v>
       </c>
-      <c r="M68" s="19" t="s">
+      <c r="M68" s="23" t="s">
         <v>308</v>
       </c>
-      <c r="N68" s="20" t="s">
+      <c r="N68" s="25" t="s">
         <v>361</v>
       </c>
       <c r="S68" s="9"/>
@@ -5631,8 +5652,8 @@
       <c r="L69" s="14">
         <v>36</v>
       </c>
-      <c r="M69" s="19"/>
-      <c r="N69" s="21"/>
+      <c r="M69" s="23"/>
+      <c r="N69" s="26"/>
       <c r="S69" s="9"/>
       <c r="T69" s="9"/>
       <c r="U69" s="9"/>
@@ -5685,10 +5706,10 @@
       <c r="L70" s="14">
         <v>37</v>
       </c>
-      <c r="M70" s="19" t="s">
+      <c r="M70" s="23" t="s">
         <v>311</v>
       </c>
-      <c r="N70" s="19" t="s">
+      <c r="N70" s="23" t="s">
         <v>312</v>
       </c>
       <c r="S70" s="9"/>
@@ -5741,8 +5762,8 @@
       <c r="L71" s="14">
         <v>38</v>
       </c>
-      <c r="M71" s="19"/>
-      <c r="N71" s="19"/>
+      <c r="M71" s="23"/>
+      <c r="N71" s="23"/>
       <c r="S71" s="9"/>
       <c r="T71" s="9"/>
       <c r="U71" s="9"/>
@@ -5793,8 +5814,8 @@
       <c r="L72" s="14">
         <v>39</v>
       </c>
-      <c r="M72" s="19"/>
-      <c r="N72" s="19"/>
+      <c r="M72" s="23"/>
+      <c r="N72" s="23"/>
       <c r="S72" s="9"/>
       <c r="T72" s="9"/>
       <c r="U72" s="9"/>
@@ -5842,8 +5863,8 @@
       <c r="L73" s="14">
         <v>40</v>
       </c>
-      <c r="M73" s="19"/>
-      <c r="N73" s="19"/>
+      <c r="M73" s="23"/>
+      <c r="N73" s="23"/>
       <c r="S73" s="9"/>
       <c r="T73" s="9"/>
       <c r="U73" s="9"/>
@@ -5884,10 +5905,10 @@
       <c r="L74" s="14">
         <v>41</v>
       </c>
-      <c r="M74" s="19" t="s">
+      <c r="M74" s="23" t="s">
         <v>311</v>
       </c>
-      <c r="N74" s="19" t="s">
+      <c r="N74" s="23" t="s">
         <v>313</v>
       </c>
       <c r="S74" s="9"/>
@@ -5930,8 +5951,8 @@
       <c r="L75" s="14">
         <v>42</v>
       </c>
-      <c r="M75" s="19"/>
-      <c r="N75" s="19"/>
+      <c r="M75" s="23"/>
+      <c r="N75" s="23"/>
       <c r="S75" s="9"/>
       <c r="T75" s="9"/>
       <c r="U75" s="9"/>
@@ -5972,8 +5993,8 @@
       <c r="L76" s="14">
         <v>43</v>
       </c>
-      <c r="M76" s="19"/>
-      <c r="N76" s="19"/>
+      <c r="M76" s="23"/>
+      <c r="N76" s="23"/>
       <c r="S76" s="9"/>
       <c r="T76" s="9"/>
       <c r="U76" s="9"/>
@@ -6014,8 +6035,8 @@
       <c r="L77" s="14">
         <v>44</v>
       </c>
-      <c r="M77" s="19"/>
-      <c r="N77" s="19"/>
+      <c r="M77" s="23"/>
+      <c r="N77" s="23"/>
       <c r="S77" s="9"/>
       <c r="T77" s="9"/>
       <c r="U77" s="9"/>
@@ -6056,10 +6077,10 @@
       <c r="L78" s="14">
         <v>45</v>
       </c>
-      <c r="M78" s="19" t="s">
+      <c r="M78" s="23" t="s">
         <v>343</v>
       </c>
-      <c r="N78" s="22" t="s">
+      <c r="N78" s="27" t="s">
         <v>362</v>
       </c>
       <c r="S78" s="9"/>
@@ -6102,8 +6123,8 @@
       <c r="L79" s="14">
         <v>46</v>
       </c>
-      <c r="M79" s="19"/>
-      <c r="N79" s="22"/>
+      <c r="M79" s="23"/>
+      <c r="N79" s="27"/>
       <c r="S79" s="9"/>
       <c r="T79" s="9"/>
       <c r="U79" s="9"/>
@@ -6138,8 +6159,8 @@
       <c r="L80" s="14">
         <v>47</v>
       </c>
-      <c r="M80" s="19"/>
-      <c r="N80" s="22"/>
+      <c r="M80" s="23"/>
+      <c r="N80" s="27"/>
       <c r="R80" s="9"/>
       <c r="S80" s="9"/>
       <c r="T80" s="9"/>
@@ -6187,8 +6208,8 @@
       <c r="L81" s="14">
         <v>48</v>
       </c>
-      <c r="M81" s="19"/>
-      <c r="N81" s="22"/>
+      <c r="M81" s="23"/>
+      <c r="N81" s="27"/>
       <c r="R81" s="9"/>
       <c r="S81" s="9"/>
       <c r="T81" s="9"/>
@@ -36731,27 +36752,6 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="L19:L23"/>
-    <mergeCell ref="M27:T28"/>
-    <mergeCell ref="M29:T30"/>
-    <mergeCell ref="L24:L26"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="M54:M55"/>
-    <mergeCell ref="N54:N55"/>
-    <mergeCell ref="N38:N39"/>
-    <mergeCell ref="N40:N41"/>
-    <mergeCell ref="M18:T18"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="M40:M41"/>
-    <mergeCell ref="M44:M47"/>
-    <mergeCell ref="N44:N47"/>
-    <mergeCell ref="M48:M51"/>
-    <mergeCell ref="N48:N51"/>
-    <mergeCell ref="M52:M53"/>
-    <mergeCell ref="N52:N53"/>
-    <mergeCell ref="M42:M43"/>
-    <mergeCell ref="N42:N43"/>
     <mergeCell ref="M68:M69"/>
     <mergeCell ref="N68:N69"/>
     <mergeCell ref="M78:M81"/>
@@ -36768,6 +36768,27 @@
     <mergeCell ref="N62:N65"/>
     <mergeCell ref="M66:M67"/>
     <mergeCell ref="N66:N67"/>
+    <mergeCell ref="M54:M55"/>
+    <mergeCell ref="N54:N55"/>
+    <mergeCell ref="N38:N39"/>
+    <mergeCell ref="N40:N41"/>
+    <mergeCell ref="M18:T18"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="M44:M47"/>
+    <mergeCell ref="N44:N47"/>
+    <mergeCell ref="M48:M51"/>
+    <mergeCell ref="N48:N51"/>
+    <mergeCell ref="M52:M53"/>
+    <mergeCell ref="N52:N53"/>
+    <mergeCell ref="M42:M43"/>
+    <mergeCell ref="N42:N43"/>
+    <mergeCell ref="L19:L23"/>
+    <mergeCell ref="M27:T28"/>
+    <mergeCell ref="M29:T30"/>
+    <mergeCell ref="L24:L26"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
   </mergeCells>
   <phoneticPr fontId="5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>